<commit_message>
final update of first part. mapping to QPX genome
</commit_message>
<xml_diff>
--- a/nodule/data/mappedNodules.xlsx
+++ b/nodule/data/mappedNodules.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162912"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
   <si>
     <t>sample</t>
   </si>
@@ -78,6 +80,39 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>pfam</t>
+  </si>
+  <si>
+    <t>peptides</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>match100</t>
+  </si>
+  <si>
+    <t>match200</t>
+  </si>
+  <si>
+    <t>match300</t>
+  </si>
+  <si>
+    <t>match400</t>
+  </si>
+  <si>
+    <t>match500</t>
+  </si>
+  <si>
+    <t>blat</t>
+  </si>
+  <si>
+    <t>assembled,contig</t>
+  </si>
+  <si>
+    <t>genomic.contig</t>
   </si>
 </sst>
 </file>
@@ -397,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -652,4 +687,355 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>498</v>
+      </c>
+      <c r="D2">
+        <v>658</v>
+      </c>
+      <c r="E2">
+        <v>1101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>359</v>
+      </c>
+      <c r="D5">
+        <v>511</v>
+      </c>
+      <c r="E5">
+        <v>1568</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1124</v>
+      </c>
+      <c r="D2">
+        <v>1111</v>
+      </c>
+      <c r="E2">
+        <v>647</v>
+      </c>
+      <c r="F2">
+        <v>382</v>
+      </c>
+      <c r="G2">
+        <v>262</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>859</v>
+      </c>
+      <c r="D5">
+        <v>831</v>
+      </c>
+      <c r="E5">
+        <v>535</v>
+      </c>
+      <c r="F5">
+        <v>342</v>
+      </c>
+      <c r="G5">
+        <v>240</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>